<commit_message>
updated to two separate tables
</commit_message>
<xml_diff>
--- a/data/criteriadata.xlsx
+++ b/data/criteriadata.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Statistics\guana\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skd09\Documents\GTM\guana\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD3A6411-F558-4046-AB39-43F2C45674EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FBE159-0E82-49A5-A72A-BDB1B560BB1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" xr2:uid="{53B5156E-1FFF-4325-8D7D-1A076751D579}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7992" activeTab="1" xr2:uid="{53B5156E-1FFF-4325-8D7D-1A076751D579}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lake" sheetId="1" r:id="rId1"/>
+    <sheet name="River" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,15 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Parameter</t>
-  </si>
-  <si>
-    <t>Lake</t>
-  </si>
-  <si>
-    <t>River</t>
   </si>
   <si>
     <t>Fecal coliform (MPN)</t>
@@ -69,12 +64,73 @@
   <si>
     <t>Dissolved Oxygen (% sat)</t>
   </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>annual geometric mean values not to be exceeded more than once in a three-year period</t>
+  </si>
+  <si>
+    <t>In no case shall nutrient concentrations of a body of water be altered so as to cause an imbalance in natural populations of aquatic flora or fauna.</t>
+  </si>
+  <si>
+    <t>counts shall not exceed 130 in 10% or more of the samples</t>
+  </si>
+  <si>
+    <r>
+      <t>The daily average percent DO saturation shall not be below 42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> percent saturation in more than 10 percent of the values</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>counts shall not exceed a median value of 14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> with not more than 10% of the samples exceeding 43</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +143,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,8 +177,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,82 +501,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24D1694-5B1C-488C-93EC-FDEEE4F73F8C}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>38</v>
-      </c>
-      <c r="C7">
-        <v>38</v>
-      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BB3A49-8B73-448A-8DAB-1E851742F26F}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>6.6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.105</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.65</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>